<commit_message>
prepare for the final release
</commit_message>
<xml_diff>
--- a/result-processed/cqrb/关键词趋势.xlsx
+++ b/result-processed/cqrb/关键词趋势.xlsx
@@ -100,8 +100,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -252,7 +255,7 @@
             <c:numRef>
               <c:f>Sheet1!$B$2:$F$2</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>6.7199999999999996E-2</c:v>
@@ -333,7 +336,7 @@
             <c:numRef>
               <c:f>Sheet1!$B$3:$F$3</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>4.0500000000000001E-2</c:v>
@@ -414,7 +417,7 @@
             <c:numRef>
               <c:f>Sheet1!$B$4:$F$4</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.04</c:v>
@@ -495,7 +498,7 @@
             <c:numRef>
               <c:f>Sheet1!$B$5:$F$5</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>2.4500000000000001E-2</c:v>
@@ -576,7 +579,7 @@
             <c:numRef>
               <c:f>Sheet1!$B$6:$F$6</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>2.1399999999999999E-2</c:v>
@@ -657,7 +660,7 @@
             <c:numRef>
               <c:f>Sheet1!$B$7:$F$7</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>2.12E-2</c:v>
@@ -740,7 +743,7 @@
             <c:numRef>
               <c:f>Sheet1!$B$8:$F$8</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>1.7399999999999999E-2</c:v>
@@ -823,7 +826,7 @@
             <c:numRef>
               <c:f>Sheet1!$B$9:$F$9</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>1.5800000000000002E-2</c:v>
@@ -906,7 +909,7 @@
             <c:numRef>
               <c:f>Sheet1!$B$10:$F$10</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>1.54E-2</c:v>
@@ -989,7 +992,7 @@
             <c:numRef>
               <c:f>Sheet1!$B$11:$F$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>1.03E-2</c:v>
@@ -1131,7 +1134,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1849,15 +1852,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>323849</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>371474</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2145,7 +2148,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2171,19 +2174,19 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>6.7199999999999996E-2</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>5.8200000000000002E-2</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>6.2600000000000003E-2</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>6.9599999999999995E-2</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="1">
         <v>6.8699999999999997E-2</v>
       </c>
     </row>
@@ -2191,19 +2194,19 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>4.0500000000000001E-2</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>4.8300000000000003E-2</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>4.2500000000000003E-2</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>4.3400000000000001E-2</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>4.2999999999999997E-2</v>
       </c>
     </row>
@@ -2211,19 +2214,19 @@
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>0.04</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>4.1799999999999997E-2</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>3.61E-2</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>4.24E-2</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1">
         <v>3.04E-2</v>
       </c>
     </row>
@@ -2231,19 +2234,19 @@
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>2.4500000000000001E-2</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>1.9300000000000001E-2</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>2.1499999999999998E-2</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>2.0899999999999998E-2</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <v>1.9699999999999999E-2</v>
       </c>
     </row>
@@ -2251,19 +2254,19 @@
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>2.1399999999999999E-2</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>1.6899999999999998E-2</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>1.55E-2</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>1.61E-2</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="1">
         <v>1.43E-2</v>
       </c>
     </row>
@@ -2271,19 +2274,19 @@
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>2.12E-2</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>1.8700000000000001E-2</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>1.7500000000000002E-2</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>1.6199999999999999E-2</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="1">
         <v>1.3599999999999999E-2</v>
       </c>
     </row>
@@ -2291,19 +2294,19 @@
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>1.7399999999999999E-2</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>1.95E-2</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>1.7100000000000001E-2</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <v>1.9099999999999999E-2</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="1">
         <v>1.32E-2</v>
       </c>
     </row>
@@ -2311,19 +2314,19 @@
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>1.5800000000000002E-2</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>1.6899999999999998E-2</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <v>1.5599999999999999E-2</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="1">
         <v>1.6E-2</v>
       </c>
     </row>
@@ -2331,19 +2334,19 @@
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>1.54E-2</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>1.5599999999999999E-2</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>1.3599999999999999E-2</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
         <v>1.3100000000000001E-2</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="1">
         <v>1.23E-2</v>
       </c>
     </row>
@@ -2351,19 +2354,19 @@
       <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>1.03E-2</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>1.09E-2</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>1.26E-2</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
         <v>9.4000000000000004E-3</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="1">
         <v>8.9999999999999993E-3</v>
       </c>
     </row>

</xml_diff>